<commit_message>
commented out python-script execution in node.js
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <bookViews>
-    <workbookView activeTab="0"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-  </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -84,11 +84,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>

</xml_diff>

<commit_message>
import to excel is a go, import from nodejs to python is a go, next step is to import to excel by increment of each cell block.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,71 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="3440" yWindow="0" windowWidth="25600" windowHeight="14960"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="1">
   <si>
-    <t>as</t>
-  </si>
-  <si>
-    <t>heyyyyyy</t>
-  </si>
-  <si>
-    <t>vfb</t>
-  </si>
-  <si>
-    <t>sef</t>
-  </si>
-  <si>
-    <t>wdef</t>
-  </si>
-  <si>
-    <t>nu</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>dgerg</t>
-  </si>
-  <si>
-    <t>grtn</t>
-  </si>
-  <si>
-    <t>fh</t>
-  </si>
-  <si>
-    <t>jgyj</t>
+    <t>['cfd893a46090']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -81,16 +55,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -415,78 +389,98 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:4">
+      <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>10</v>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="D11" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
able to insert data to cell and then increment by one. Each scan will be add to a cell in Excel
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,45 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <bookViews>
-    <workbookView xWindow="3440" yWindow="0" windowWidth="25600" windowHeight="14960"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr codeName="ThisWorkbook"/>
+  <s:bookViews>
+    <s:workbookView activeTab="0"/>
+  </s:bookViews>
+  <s:sheets>
+    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </s:sheets>
+  <s:definedNames/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
+</s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
   <si>
-    <t>['cfd893a46090']</t>
+    <t>['8a9ab3409000']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -54,17 +64,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="3">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="3">
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -389,98 +403,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="D11" t="s">
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deleted node.js code. Added Python pycard code.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -6,7 +6,7 @@
     <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,9 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
-    <t>['8a9ab3409000']</t>
+    <t>CFD893A460</t>
+  </si>
+  <si>
+    <t>gary tsai</t>
+  </si>
+  <si>
+    <t>8A9AB340</t>
+  </si>
+  <si>
+    <t>CBS</t>
   </si>
 </sst>
 </file>
@@ -24,7 +33,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -64,18 +80,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+  <cellStyleXfs count="18">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="18">
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 6" xfId="2"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
+    <cellStyle builtinId="0" name="Normal" xfId="4"/>
+    <cellStyle name="Normal 3" xfId="5"/>
+    <cellStyle name="Normal 11" xfId="6"/>
+    <cellStyle name="Normal 10" xfId="7"/>
+    <cellStyle name="Normal 13" xfId="8"/>
+    <cellStyle name="Normal 12" xfId="9"/>
+    <cellStyle name="Normal 5" xfId="10"/>
+    <cellStyle name="Normal 14" xfId="11"/>
+    <cellStyle name="Normal 7" xfId="12"/>
+    <cellStyle name="Normal 16" xfId="13"/>
+    <cellStyle name="Normal 9" xfId="14"/>
+    <cellStyle name="Normal 8" xfId="15"/>
+    <cellStyle name="Normal 15" xfId="16"/>
+    <cellStyle name="Normal 4" xfId="17"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -408,37 +454,35 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:1">
+    <row r="1" spans="1:3"/>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added auto email and Hashing function
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -7,6 +7,7 @@
   </s:bookViews>
   <s:sheets>
     <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Monthly_STAT" sheetId="2" r:id="rId2"/>
   </s:sheets>
   <s:definedNames/>
   <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,18 +15,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
+  <si>
+    <t>8A9AB340</t>
+  </si>
+  <si>
+    <t>CBS</t>
+  </si>
   <si>
     <t>CFD893A460</t>
   </si>
   <si>
-    <t>gary tsai</t>
-  </si>
-  <si>
-    <t>8A9AB340</t>
-  </si>
-  <si>
-    <t>CBS</t>
+    <t>Gary Tsai</t>
+  </si>
+  <si>
+    <t>8FD8AAE4A0</t>
+  </si>
+  <si>
+    <t>Steven Vargas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total student visited this month: </t>
   </si>
 </sst>
 </file>
@@ -33,7 +43,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -61,6 +71,34 @@
       <color theme="10"/>
       <sz val="12"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <i val="1"/>
+      <color rgb="FF000000"/>
+      <sz val="18"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="11"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <i val="1"/>
+      <color rgb="00000000"/>
+      <sz val="18"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,11 +118,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="18">
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+  <cellStyleXfs count="19">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -100,28 +139,31 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="14"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="14"/>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="19">
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 6" xfId="2"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
-    <cellStyle builtinId="0" name="Normal" xfId="4"/>
-    <cellStyle name="Normal 3" xfId="5"/>
-    <cellStyle name="Normal 11" xfId="6"/>
-    <cellStyle name="Normal 10" xfId="7"/>
-    <cellStyle name="Normal 13" xfId="8"/>
-    <cellStyle name="Normal 12" xfId="9"/>
-    <cellStyle name="Normal 5" xfId="10"/>
-    <cellStyle name="Normal 14" xfId="11"/>
-    <cellStyle name="Normal 7" xfId="12"/>
-    <cellStyle name="Normal 16" xfId="13"/>
-    <cellStyle name="Normal 9" xfId="14"/>
-    <cellStyle name="Normal 8" xfId="15"/>
-    <cellStyle name="Normal 15" xfId="16"/>
-    <cellStyle name="Normal 4" xfId="17"/>
+    <cellStyle name="Normal 17" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="2"/>
+    <cellStyle name="Normal 16" xfId="3"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="4"/>
+    <cellStyle name="Normal 13" xfId="5"/>
+    <cellStyle name="Normal 14" xfId="6"/>
+    <cellStyle name="Normal 11" xfId="7"/>
+    <cellStyle name="Normal 10" xfId="8"/>
+    <cellStyle name="Normal 3" xfId="9"/>
+    <cellStyle name="Normal 12" xfId="10"/>
+    <cellStyle name="Normal 5" xfId="11"/>
+    <cellStyle name="Normal 2" xfId="12"/>
+    <cellStyle name="Normal 7" xfId="13"/>
+    <cellStyle name="Normal 6" xfId="14"/>
+    <cellStyle name="Normal 9" xfId="15"/>
+    <cellStyle name="Normal 8" xfId="16"/>
+    <cellStyle name="Normal 15" xfId="17"/>
+    <cellStyle name="Normal 4" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -454,10 +496,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -471,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row customHeight="1" ht="30" r="3" spans="1:3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -482,7 +524,47 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="4294967292" orientation="portrait" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row customHeight="1" ht="23" r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <f>SUM(sheet!C2:C4)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added card verification and ASCII art
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>UID</t>
   </si>
@@ -42,6 +42,51 @@
   </si>
   <si>
     <t>Steven Vargas</t>
+  </si>
+  <si>
+    <t>01FE5197502AC472</t>
+  </si>
+  <si>
+    <t>S4 phone</t>
+  </si>
+  <si>
+    <t>00000000</t>
+  </si>
+  <si>
+    <t>s4.2</t>
+  </si>
+  <si>
+    <t>08CE7849</t>
+  </si>
+  <si>
+    <t>08A088E0</t>
+  </si>
+  <si>
+    <t>hello there</t>
+  </si>
+  <si>
+    <t>08AB5506</t>
+  </si>
+  <si>
+    <t>lklk</t>
+  </si>
+  <si>
+    <t>089BFDF0</t>
+  </si>
+  <si>
+    <t>gary</t>
+  </si>
+  <si>
+    <t>082881DB</t>
+  </si>
+  <si>
+    <t>nihao</t>
+  </si>
+  <si>
+    <t>01FE940C1FD75197</t>
+  </si>
+  <si>
+    <t>ni</t>
   </si>
   <si>
     <t>Total visits this month:</t>
@@ -512,7 +557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
@@ -546,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>82</v>
+        <v>117</v>
       </c>
     </row>
     <row customHeight="1" ht="30" r="3" spans="1:5">
@@ -557,7 +602,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -569,6 +614,94 @@
       </c>
       <c r="C4" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -593,10 +726,10 @@
   <sheetData>
     <row customHeight="1" ht="23" r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
-        <f>SUM(sheet!E2:E4)</f>
+        <f>SUM(sheet!E2:E12)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
added ASCII art to alert.py
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -183,8 +183,8 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -208,17 +208,17 @@
   <cellStyles count="19">
     <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
     <cellStyle name="Normal 17" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="2"/>
-    <cellStyle name="Normal 16" xfId="3"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="4"/>
-    <cellStyle name="Normal 13" xfId="5"/>
-    <cellStyle name="Normal 14" xfId="6"/>
+    <cellStyle name="Normal 12" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="3"/>
+    <cellStyle name="Normal 16" xfId="4"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
+    <cellStyle name="Normal 13" xfId="6"/>
     <cellStyle name="Normal 11" xfId="7"/>
     <cellStyle name="Normal 10" xfId="8"/>
     <cellStyle name="Normal 3" xfId="9"/>
-    <cellStyle name="Normal 12" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="10"/>
     <cellStyle name="Normal 5" xfId="11"/>
-    <cellStyle name="Normal 2" xfId="12"/>
+    <cellStyle name="Normal 14" xfId="12"/>
     <cellStyle name="Normal 7" xfId="13"/>
     <cellStyle name="Normal 6" xfId="14"/>
     <cellStyle name="Normal 9" xfId="15"/>
@@ -591,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>117</v>
+        <v>153</v>
       </c>
     </row>
     <row customHeight="1" ht="30" r="3" spans="1:5">

</xml_diff>

<commit_message>
first change in deploy mac
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>UID</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>August 2016</t>
+  </si>
+  <si>
     <t>CFD893A460</t>
   </si>
   <si>
@@ -45,6 +48,60 @@
   </si>
   <si>
     <t>CBS</t>
+  </si>
+  <si>
+    <t>CFD8A78940</t>
+  </si>
+  <si>
+    <t>Nicole Latta</t>
+  </si>
+  <si>
+    <t>8FD8940860</t>
+  </si>
+  <si>
+    <t>David schachner</t>
+  </si>
+  <si>
+    <t>0FD8A9BD80</t>
+  </si>
+  <si>
+    <t>Jaspreet Kaur</t>
+  </si>
+  <si>
+    <t>CFD8A9E820</t>
+  </si>
+  <si>
+    <t>Richard Pusateri</t>
+  </si>
+  <si>
+    <t>0FD8A82F40</t>
+  </si>
+  <si>
+    <t>Mario Regino</t>
+  </si>
+  <si>
+    <t>CFD8AA9A20</t>
+  </si>
+  <si>
+    <t>Randell Holland</t>
+  </si>
+  <si>
+    <t>CFD89A9C80</t>
+  </si>
+  <si>
+    <t>Bryan Williams</t>
+  </si>
+  <si>
+    <t>4FD8A85BA0</t>
+  </si>
+  <si>
+    <t>Hojin Euam</t>
+  </si>
+  <si>
+    <t>0FD8A290A0</t>
+  </si>
+  <si>
+    <t>Paul Fabro</t>
   </si>
   <si>
     <t>Total visits this month:</t>
@@ -132,17 +189,17 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -157,25 +214,25 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="10"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="2"/>
-    <cellStyle name="Normal 17" xfId="3"/>
-    <cellStyle name="Normal 7" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normal 6" xfId="6"/>
-    <cellStyle name="Normal 8" xfId="7"/>
-    <cellStyle name="Normal 15" xfId="8"/>
-    <cellStyle name="Normal 12" xfId="9"/>
-    <cellStyle name="Normal 10" xfId="10"/>
-    <cellStyle name="Normal 11" xfId="11"/>
-    <cellStyle name="Normal 14" xfId="12"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="13"/>
-    <cellStyle name="Normal 2" xfId="14"/>
-    <cellStyle name="Normal 13" xfId="15"/>
-    <cellStyle name="Normal 5" xfId="16"/>
+    <cellStyle name="Normal 3" xfId="0"/>
+    <cellStyle name="Normal 4" xfId="1"/>
+    <cellStyle name="Normal 8" xfId="2"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
+    <cellStyle name="Normal 5" xfId="4"/>
+    <cellStyle name="Normal 10" xfId="5"/>
+    <cellStyle name="Normal 15" xfId="6"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="7"/>
+    <cellStyle builtinId="0" name="Normal" xfId="8"/>
+    <cellStyle name="Normal 13" xfId="9"/>
+    <cellStyle name="Normal 12" xfId="10"/>
+    <cellStyle name="Normal 17" xfId="11"/>
+    <cellStyle name="Normal 2" xfId="12"/>
+    <cellStyle name="Normal 14" xfId="13"/>
+    <cellStyle name="Normal 6" xfId="14"/>
+    <cellStyle name="Normal 7" xfId="15"/>
+    <cellStyle name="Normal 9" xfId="16"/>
     <cellStyle name="Normal 16" xfId="17"/>
-    <cellStyle name="Normal 9" xfId="18"/>
+    <cellStyle name="Normal 11" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -508,7 +565,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -520,56 +577,161 @@
     <col customWidth="1" max="2" min="2" width="20"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23" r="1" spans="1:3">
+    <row customHeight="1" ht="23" r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row customHeight="1" ht="30" r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="30" r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="n">
-        <v>9</v>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -594,12 +756,9 @@
   <sheetData>
     <row customHeight="1" ht="23" r="3" spans="1:3">
       <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4">
-        <f>SUM(sheet!C2:C5)</f>
-        <v/>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
added email festure to spreadsheet
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>UID</t>
   </si>
@@ -23,6 +23,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>August 2016</t>
   </si>
   <si>
@@ -92,16 +95,22 @@
     <t>Paul Fabro</t>
   </si>
   <si>
-    <t>8A9AB340</t>
-  </si>
-  <si>
-    <t>CBS</t>
-  </si>
-  <si>
     <t>CFD893A460</t>
   </si>
   <si>
-    <t>Gary Tsai</t>
+    <t>garytsai</t>
+  </si>
+  <si>
+    <t>garytsai@live</t>
+  </si>
+  <si>
+    <t>4FD87D1F40</t>
+  </si>
+  <si>
+    <t>Gao Fang</t>
+  </si>
+  <si>
+    <t>fang.gao@jjay.cuny.edu</t>
   </si>
   <si>
     <t>Month</t>
@@ -144,15 +153,15 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <i val="1"/>
       <color rgb="FF000000"/>
-      <sz val="18"/>
+      <sz val="15"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <i val="1"/>
       <color rgb="FF000000"/>
-      <sz val="15"/>
+      <sz val="18"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -184,47 +193,49 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="18"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="10"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="18"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="6"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="12"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="16"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="12"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="16"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 17" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="3"/>
-    <cellStyle name="Normal 16" xfId="4"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
-    <cellStyle name="Normal 13" xfId="6"/>
-    <cellStyle name="Normal 11" xfId="7"/>
-    <cellStyle name="Normal 10" xfId="8"/>
-    <cellStyle name="Normal 3" xfId="9"/>
-    <cellStyle name="Normal 12" xfId="10"/>
-    <cellStyle name="Normal 5" xfId="11"/>
-    <cellStyle name="Normal 4" xfId="12"/>
-    <cellStyle name="Normal 7" xfId="13"/>
-    <cellStyle name="Normal 6" xfId="14"/>
-    <cellStyle name="Normal 9" xfId="15"/>
+    <cellStyle name="Normal 11" xfId="0"/>
+    <cellStyle name="Normal 16" xfId="1"/>
+    <cellStyle name="Normal 14" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="4"/>
+    <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 10" xfId="6"/>
+    <cellStyle name="Normal 5" xfId="7"/>
+    <cellStyle name="Normal 15" xfId="8"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="9"/>
+    <cellStyle builtinId="0" name="Normal" xfId="10"/>
+    <cellStyle name="Normal 6" xfId="11"/>
+    <cellStyle name="Normal 9" xfId="12"/>
+    <cellStyle name="Normal 13" xfId="13"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="14"/>
+    <cellStyle name="Normal 17" xfId="15"/>
     <cellStyle name="Normal 8" xfId="16"/>
-    <cellStyle name="Normal 15" xfId="17"/>
-    <cellStyle name="Normal 14" xfId="18"/>
+    <cellStyle name="Normal 7" xfId="17"/>
+    <cellStyle name="Normal 12" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -557,10 +568,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -568,127 +579,137 @@
     <col customWidth="1" max="4" min="1" width="20"/>
     <col customWidth="1" max="2" min="2" width="20"/>
     <col customWidth="1" max="3" min="3" width="20"/>
+    <col customWidth="1" max="4" min="4" width="20"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23" r="1" spans="1:3">
-      <c r="A1" s="3" t="s">
+    <row customHeight="1" ht="23" r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="n">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -715,16 +736,16 @@
   </cols>
   <sheetData>
     <row customHeight="1" ht="19" r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>29</v>
+      <c r="A1" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <f>SUM(Sheet!C2:C14)</f>
+        <f>SUM(Sheet!D2:D14)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed print statment on searchStudeny.py
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
   <si>
     <t>UID</t>
   </si>
@@ -59,6 +59,9 @@
     <t>Jaspreet Kaur</t>
   </si>
   <si>
+    <t>jaspreet.kaur6@jjay.cuny.edu</t>
+  </si>
+  <si>
     <t>CFD8A9E820</t>
   </si>
   <si>
@@ -74,7 +77,10 @@
     <t>CFD8AA9A20</t>
   </si>
   <si>
-    <t>Randell Holland</t>
+    <t>Rondell Holland</t>
+  </si>
+  <si>
+    <t>rondell.holland@jjay.cuny.edu</t>
   </si>
   <si>
     <t>CFD89A9C80</t>
@@ -111,6 +117,24 @@
   </si>
   <si>
     <t>fang.gao@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>8FD8A841E0</t>
+  </si>
+  <si>
+    <t>Sujay Bhaskar kashyap</t>
+  </si>
+  <si>
+    <t>sujay.bhaskarkashyap@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>8FD8AC0500</t>
+  </si>
+  <si>
+    <t>jimmy Barreto</t>
+  </si>
+  <si>
+    <t>j.barreto1823@yahoo.com</t>
   </si>
   <si>
     <t>Month</t>
@@ -188,21 +212,21 @@
     </border>
   </borders>
   <cellStyleXfs count="19">
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
@@ -217,25 +241,25 @@
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="16"/>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="Normal 11" xfId="0"/>
-    <cellStyle name="Normal 16" xfId="1"/>
-    <cellStyle name="Normal 14" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
-    <cellStyle name="Normal 2" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normal 10" xfId="6"/>
-    <cellStyle name="Normal 5" xfId="7"/>
-    <cellStyle name="Normal 15" xfId="8"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="9"/>
-    <cellStyle builtinId="0" name="Normal" xfId="10"/>
-    <cellStyle name="Normal 6" xfId="11"/>
-    <cellStyle name="Normal 9" xfId="12"/>
-    <cellStyle name="Normal 13" xfId="13"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="14"/>
-    <cellStyle name="Normal 17" xfId="15"/>
-    <cellStyle name="Normal 8" xfId="16"/>
-    <cellStyle name="Normal 7" xfId="17"/>
-    <cellStyle name="Normal 12" xfId="18"/>
+    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="0"/>
+    <cellStyle name="Normal 10" xfId="1"/>
+    <cellStyle name="Normal 5" xfId="2"/>
+    <cellStyle name="Normal 17" xfId="3"/>
+    <cellStyle name="Normal 13" xfId="4"/>
+    <cellStyle name="Normal 9" xfId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="6"/>
+    <cellStyle name="Normal 4" xfId="7"/>
+    <cellStyle name="Normal 11" xfId="8"/>
+    <cellStyle name="Normal 2" xfId="9"/>
+    <cellStyle name="Normal 7" xfId="10"/>
+    <cellStyle name="Normal 12" xfId="11"/>
+    <cellStyle name="Normal 8" xfId="12"/>
+    <cellStyle name="Normal 15" xfId="13"/>
+    <cellStyle name="Normal 14" xfId="14"/>
+    <cellStyle name="Normal 6" xfId="15"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="16"/>
+    <cellStyle name="Normal 3" xfId="17"/>
+    <cellStyle name="Normal 16" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -568,7 +592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -635,81 +659,121 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -737,7 +801,7 @@
   <sheetData>
     <row customHeight="1" ht="19" r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -745,7 +809,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <f>SUM(Sheet!D2:D14)</f>
+        <f>SUM(Sheet!D2:D16)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
testing reporting.py for logs feature.
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>UID</t>
   </si>
@@ -135,6 +135,30 @@
   </si>
   <si>
     <t>j.barreto1823@yahoo.com</t>
+  </si>
+  <si>
+    <t>saergetsrt</t>
+  </si>
+  <si>
+    <t>saeccffrgetsrt</t>
+  </si>
+  <si>
+    <t>gary</t>
+  </si>
+  <si>
+    <t>@live</t>
+  </si>
+  <si>
+    <t>saeccffrgeaa</t>
+  </si>
+  <si>
+    <t>Gary Tsai</t>
+  </si>
+  <si>
+    <t>yue.tsai@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>saeccffrgea</t>
   </si>
   <si>
     <t>Month</t>
@@ -145,7 +169,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -187,12 +211,6 @@
       <color rgb="FF000000"/>
       <sz val="18"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="18"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -232,34 +250,32 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="6"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="12"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="16"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="12"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="16"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="3"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="15"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 5" xfId="2"/>
-    <cellStyle name="Normal 17" xfId="3"/>
-    <cellStyle name="Normal 13" xfId="4"/>
-    <cellStyle name="Normal 9" xfId="5"/>
-    <cellStyle builtinId="0" name="Normal" xfId="6"/>
+    <cellStyle name="Normal 9" xfId="1"/>
+    <cellStyle name="Normal 6" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 14" xfId="4"/>
+    <cellStyle name="Normal 15" xfId="5"/>
+    <cellStyle name="Normal 12" xfId="6"/>
     <cellStyle name="Normal 4" xfId="7"/>
-    <cellStyle name="Normal 11" xfId="8"/>
-    <cellStyle name="Normal 2" xfId="9"/>
-    <cellStyle name="Normal 7" xfId="10"/>
-    <cellStyle name="Normal 12" xfId="11"/>
-    <cellStyle name="Normal 8" xfId="12"/>
-    <cellStyle name="Normal 15" xfId="13"/>
-    <cellStyle name="Normal 14" xfId="14"/>
-    <cellStyle name="Normal 6" xfId="15"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="16"/>
+    <cellStyle builtinId="0" name="Normal" xfId="8"/>
+    <cellStyle name="Normal 7" xfId="9"/>
+    <cellStyle name="Normal 5" xfId="10"/>
+    <cellStyle name="Normal 13" xfId="11"/>
+    <cellStyle name="Normal 10" xfId="12"/>
+    <cellStyle name="Normal 8" xfId="13"/>
+    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="14"/>
+    <cellStyle name="Normal 16" xfId="15"/>
+    <cellStyle name="Normal 11" xfId="16"/>
     <cellStyle name="Normal 3" xfId="17"/>
-    <cellStyle name="Normal 16" xfId="18"/>
+    <cellStyle name="Normal 17" xfId="18"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -592,28 +608,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="4" min="1" width="20"/>
-    <col customWidth="1" max="2" min="2" width="20"/>
-    <col customWidth="1" max="3" min="3" width="20"/>
-    <col customWidth="1" max="4" min="4" width="20"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="23" r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -774,6 +787,52 @@
       </c>
       <c r="D16" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s"/>
+      <c r="C20" t="s"/>
+      <c r="D20" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -788,7 +847,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -799,18 +858,14 @@
     <col customWidth="1" max="1" min="1" width="25"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="19" r="1" spans="1:2">
+    <row customHeight="1" ht="19" r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2">
-        <f>SUM(Sheet!D2:D16)</f>
-        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed to match desktop
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Monthly_STAT" sheetId="2" r:id="rId2"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthly_STAT" sheetId="2" r:id="rId2"/>
+  </sheets>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="323">
   <si>
     <t>UID</t>
   </si>
@@ -59,7 +64,10 @@
     <t>8FD8940860</t>
   </si>
   <si>
-    <t>David schachner</t>
+    <t>David Schachner</t>
+  </si>
+  <si>
+    <t>david.schachner@jjay.cuny.edu</t>
   </si>
   <si>
     <t>0FD8A9BD80</t>
@@ -86,7 +94,10 @@
     <t>CFD8AA9A20</t>
   </si>
   <si>
-    <t>Randell Holland</t>
+    <t>Rondell Holland</t>
+  </si>
+  <si>
+    <t>rondell.holland@jjay.cuny.edu</t>
   </si>
   <si>
     <t>CFD89A9C80</t>
@@ -95,6 +106,9 @@
     <t>Bryan Williams</t>
   </si>
   <si>
+    <t>bryan.williams@jjay.cuny.edu</t>
+  </si>
+  <si>
     <t>4FD8A85BA0</t>
   </si>
   <si>
@@ -110,12 +124,12 @@
     <t>Paul Fabro</t>
   </si>
   <si>
+    <t>paul.fabro@jjay.cuny.edu</t>
+  </si>
+  <si>
     <t>8A9AB340</t>
   </si>
   <si>
-    <t>gary</t>
-  </si>
-  <si>
     <t>CFD893A460</t>
   </si>
   <si>
@@ -873,6 +887,105 @@
   </si>
   <si>
     <t>megan.eng@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>8FD8A841E0</t>
+  </si>
+  <si>
+    <t>Sujay Bhaskar KashYap</t>
+  </si>
+  <si>
+    <t>sujay.bhaskarkashyap@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>CFD8ADF120</t>
+  </si>
+  <si>
+    <t>8FD8AC1E00</t>
+  </si>
+  <si>
+    <t>8FD8967BC0</t>
+  </si>
+  <si>
+    <t>Israel Matos</t>
+  </si>
+  <si>
+    <t>israel.matos@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>4FD8A9E700</t>
+  </si>
+  <si>
+    <t>Nicole Cintron</t>
+  </si>
+  <si>
+    <t>nicole.cintron@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>0FD8A51D80</t>
+  </si>
+  <si>
+    <t>Miguelina Garcia</t>
+  </si>
+  <si>
+    <t>miguelina.garcia@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>0FD8AD42A0</t>
+  </si>
+  <si>
+    <t>Covalky Pena</t>
+  </si>
+  <si>
+    <t>covalky.pena@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>CFD8A00C40</t>
+  </si>
+  <si>
+    <t>nadinemay espinosa</t>
+  </si>
+  <si>
+    <t>nadinemay.espinosa@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>CFD8A0E820</t>
+  </si>
+  <si>
+    <t>SAMUEL TORRES</t>
+  </si>
+  <si>
+    <t>SAMUEL.TORRES@JJAY.CUNY.EDU</t>
+  </si>
+  <si>
+    <t>8FD8AC5D40</t>
+  </si>
+  <si>
+    <t>Rudelina Calcano</t>
+  </si>
+  <si>
+    <t>rudelina.calcano@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>8FD8ACC280</t>
+  </si>
+  <si>
+    <t>Emmanuel Macintosh</t>
+  </si>
+  <si>
+    <t>emmanuel.mcintosh@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>8FD894EAC0</t>
+  </si>
+  <si>
+    <t>Sade Thomas</t>
+  </si>
+  <si>
+    <t>sade.thomas@jjay.cuny.edu</t>
+  </si>
+  <si>
+    <t>0FD8AE0B20</t>
   </si>
   <si>
     <t>Month</t>
@@ -881,45 +994,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color indexed="8"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="18"/>
     </font>
     <font>
+      <i/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <i val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="15"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="18"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <i val="1"/>
-      <color rgb="00000000"/>
-      <sz val="15"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -956,25 +1055,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="49" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="17" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="49" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2150,35 +2246,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IL113"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="20"/>
-    <col customWidth="1" max="3" min="2" style="4" width="30"/>
-    <col customWidth="1" max="3" min="3" style="4" width="30"/>
-    <col customWidth="1" max="238" min="4" style="4" width="20"/>
-    <col customWidth="1" max="6" min="6" style="4" width="20"/>
-    <col customWidth="1" max="7" min="7" style="4" width="20"/>
+    <col min="1" max="1" width="20" style="4" customWidth="1"/>
+    <col min="2" max="3" width="30" style="4" customWidth="1"/>
+    <col min="4" max="246" width="20" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23" r="1" s="4" spans="1:7">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" ht="23" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2187,24 +2276,18 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="2" s="4" spans="1:7">
+    </row>
+    <row r="2" spans="1:5" ht="17" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="3" s="4" spans="1:7">
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -2214,11 +2297,11 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="4" s="4" spans="1:7">
+      <c r="D3" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -2228,1359 +2311,1527 @@
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="5" s="4" spans="1:7">
+    <row r="5" spans="1:5" ht="17" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="n"/>
-      <c r="D5" s="3" t="n">
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="6" s="4" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="n">
+    <row r="8" spans="1:5" ht="17" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="17" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="3">
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="7" s="4" spans="1:7">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n">
+    <row r="13" spans="1:5" ht="17" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="8" s="4" spans="1:7">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="9" s="4" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" s="2" t="n">
+    <row r="14" spans="1:5" ht="17" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="10" s="4" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="n">
+    <row r="21" spans="1:4" ht="17" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="2">
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="11" s="4" spans="1:7">
-      <c r="A11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="2" t="n">
+    <row r="22" spans="1:4" ht="17" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="2">
         <v>9</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="12" s="4" spans="1:7">
-      <c r="A12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="13" s="4" spans="1:7">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="3" t="n">
+    <row r="28" spans="1:4" ht="17" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="2">
         <v>4</v>
       </c>
-      <c r="F13" t="n">
+    </row>
+    <row r="30" spans="1:4" ht="17" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="2">
         <v>1</v>
       </c>
-      <c r="G13" t="n">
+    </row>
+    <row r="34" spans="1:4" ht="17" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" customHeight="1">
+      <c r="A37" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" customHeight="1">
+      <c r="A38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" customHeight="1">
+      <c r="A40" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="2">
         <v>2</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="14" s="4" spans="1:7">
-      <c r="A14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="15" s="4" spans="1:7">
-      <c r="A15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="2" t="n">
+    <row r="42" spans="1:4" ht="17" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" customHeight="1">
+      <c r="A43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" customHeight="1">
+      <c r="A45" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" customHeight="1">
+      <c r="A46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D49" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D50" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D51" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="17" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="17" customHeight="1">
+      <c r="A53" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="17" customHeight="1">
+      <c r="A54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="17" customHeight="1">
+      <c r="A55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17" customHeight="1">
+      <c r="A56" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D56" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="17" customHeight="1">
+      <c r="A57" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D57" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="17" customHeight="1">
+      <c r="A58" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="17" customHeight="1">
+      <c r="A59" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D59" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="17" customHeight="1">
+      <c r="A60" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="17" customHeight="1">
+      <c r="A61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D61" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="17" customHeight="1">
+      <c r="A62" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="17" customHeight="1">
+      <c r="A63" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D63" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="17" customHeight="1">
+      <c r="A64" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="17" customHeight="1">
+      <c r="A65" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D65" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17" customHeight="1">
+      <c r="A66" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D66" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" t="s">
+        <v>196</v>
+      </c>
+      <c r="B68" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>199</v>
+      </c>
+      <c r="B69" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" t="s">
+        <v>201</v>
+      </c>
+      <c r="D69">
         <v>8</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="16" s="4" spans="1:7">
-      <c r="A16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="2" t="n">
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>202</v>
+      </c>
+      <c r="B70" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" t="s">
+        <v>204</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" t="s">
+        <v>208</v>
+      </c>
+      <c r="B72" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" t="s">
+        <v>210</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" t="s">
+        <v>211</v>
+      </c>
+      <c r="B73" t="s">
+        <v>212</v>
+      </c>
+      <c r="C73" t="s">
+        <v>213</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" t="s">
+        <v>214</v>
+      </c>
+      <c r="B74" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" t="s">
+        <v>217</v>
+      </c>
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" t="s">
+        <v>220</v>
+      </c>
+      <c r="B76" t="s">
+        <v>221</v>
+      </c>
+      <c r="C76" t="s">
+        <v>222</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" t="s">
+        <v>226</v>
+      </c>
+      <c r="B78" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" t="s">
+        <v>228</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
+        <v>229</v>
+      </c>
+      <c r="B79" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" t="s">
+        <v>231</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" t="s">
+        <v>232</v>
+      </c>
+      <c r="B80" t="s">
+        <v>233</v>
+      </c>
+      <c r="C80" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" t="s">
+        <v>235</v>
+      </c>
+      <c r="B81" t="s">
+        <v>236</v>
+      </c>
+      <c r="C81" t="s">
+        <v>237</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>238</v>
+      </c>
+      <c r="B82" t="s">
+        <v>239</v>
+      </c>
+      <c r="C82" t="s">
+        <v>240</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" t="s">
+        <v>241</v>
+      </c>
+      <c r="B83" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" t="s">
+        <v>243</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
+        <v>244</v>
+      </c>
+      <c r="B84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C84" t="s">
+        <v>246</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" t="s">
+        <v>247</v>
+      </c>
+      <c r="B85" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" t="s">
+        <v>249</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
+        <v>250</v>
+      </c>
+      <c r="B86" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" t="s">
+        <v>252</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>253</v>
+      </c>
+      <c r="B87" t="s">
+        <v>254</v>
+      </c>
+      <c r="C87" t="s">
+        <v>255</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
+        <v>256</v>
+      </c>
+      <c r="B88" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" t="s">
+        <v>258</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" t="s">
+        <v>259</v>
+      </c>
+      <c r="B89" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" t="s">
+        <v>261</v>
+      </c>
+      <c r="D89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
+        <v>262</v>
+      </c>
+      <c r="B90" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" t="s">
+        <v>264</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>265</v>
+      </c>
+      <c r="B91" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D91">
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="17" s="4" spans="1:7">
-      <c r="A17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="2" t="n">
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
+        <v>268</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" t="s">
+        <v>269</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" t="s">
+        <v>270</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" t="s">
+        <v>271</v>
+      </c>
+      <c r="B95" t="s">
+        <v>272</v>
+      </c>
+      <c r="C95" t="s">
+        <v>273</v>
+      </c>
+      <c r="D95">
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="18" s="4" spans="1:7">
-      <c r="A18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="19" s="4" spans="1:7">
-      <c r="A19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="2" t="n">
+    <row r="96" spans="1:4">
+      <c r="A96" t="s">
+        <v>274</v>
+      </c>
+      <c r="B96" t="s">
+        <v>275</v>
+      </c>
+      <c r="C96" t="s">
+        <v>276</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>277</v>
+      </c>
+      <c r="B97" t="s">
+        <v>278</v>
+      </c>
+      <c r="C97" t="s">
+        <v>279</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" t="s">
+        <v>280</v>
+      </c>
+      <c r="B98" t="s">
+        <v>281</v>
+      </c>
+      <c r="C98" t="s">
+        <v>282</v>
+      </c>
+      <c r="D98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
+        <v>283</v>
+      </c>
+      <c r="B99" t="s">
+        <v>284</v>
+      </c>
+      <c r="C99" t="s">
+        <v>285</v>
+      </c>
+      <c r="D99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>286</v>
+      </c>
+      <c r="B100" t="s">
+        <v>287</v>
+      </c>
+      <c r="C100" t="s">
+        <v>288</v>
+      </c>
+      <c r="D100">
         <v>3</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="20" s="4" spans="1:7">
-      <c r="A20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="3" t="n"/>
-      <c r="D20" s="2" t="n">
+    <row r="101" spans="1:4">
+      <c r="A101" t="s">
+        <v>289</v>
+      </c>
+      <c r="B101" t="s">
+        <v>290</v>
+      </c>
+      <c r="C101" t="s">
+        <v>291</v>
+      </c>
+      <c r="D101">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="21" s="4" spans="1:7">
-      <c r="A21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="2" t="n">
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>292</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" t="s">
+        <v>293</v>
+      </c>
+      <c r="D103">
         <v>4</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="22" s="4" spans="1:7">
-      <c r="A22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="23" s="4" spans="1:7">
-      <c r="A23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="24" s="4" spans="1:7">
-      <c r="A24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="25" s="4" spans="1:7">
-      <c r="A25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="2" t="n">
+    <row r="104" spans="1:4">
+      <c r="A104" t="s">
+        <v>294</v>
+      </c>
+      <c r="B104" t="s">
+        <v>295</v>
+      </c>
+      <c r="C104" t="s">
+        <v>296</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" t="s">
+        <v>297</v>
+      </c>
+      <c r="B105" t="s">
+        <v>298</v>
+      </c>
+      <c r="C105" t="s">
+        <v>299</v>
+      </c>
+      <c r="D105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>300</v>
+      </c>
+      <c r="B106" t="s">
+        <v>301</v>
+      </c>
+      <c r="C106" t="s">
+        <v>302</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>303</v>
+      </c>
+      <c r="B107" t="s">
+        <v>304</v>
+      </c>
+      <c r="C107" t="s">
+        <v>305</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>306</v>
+      </c>
+      <c r="B108" t="s">
+        <v>307</v>
+      </c>
+      <c r="C108" t="s">
+        <v>308</v>
+      </c>
+      <c r="D108">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>309</v>
+      </c>
+      <c r="B109" t="s">
+        <v>310</v>
+      </c>
+      <c r="C109" t="s">
+        <v>311</v>
+      </c>
+      <c r="D109">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="26" s="4" spans="1:7">
-      <c r="A26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="2" t="n">
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>312</v>
+      </c>
+      <c r="B110" t="s">
+        <v>313</v>
+      </c>
+      <c r="C110" t="s">
+        <v>314</v>
+      </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>315</v>
+      </c>
+      <c r="B111" t="s">
+        <v>316</v>
+      </c>
+      <c r="C111" t="s">
+        <v>317</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>318</v>
+      </c>
+      <c r="B112" t="s">
+        <v>319</v>
+      </c>
+      <c r="C112" t="s">
+        <v>320</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>321</v>
+      </c>
+      <c r="D113">
         <v>1</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="27" s="4" spans="1:7">
-      <c r="A27" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="28" s="4" spans="1:7">
-      <c r="A28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="29" s="4" spans="1:7">
-      <c r="A29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="30" s="4" spans="1:7">
-      <c r="A30" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="31" s="4" spans="1:7">
-      <c r="A31" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="32" s="4" spans="1:7">
-      <c r="A32" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="33" s="4" spans="1:7">
-      <c r="A33" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="34" s="4" spans="1:7">
-      <c r="A34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="35" s="4" spans="1:7">
-      <c r="A35" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="36" s="4" spans="1:7">
-      <c r="A36" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="37" s="4" spans="1:7">
-      <c r="A37" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="38" s="4" spans="1:7">
-      <c r="A38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="39" s="4" spans="1:7">
-      <c r="A39" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="40" s="4" spans="1:7">
-      <c r="A40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="41" s="4" spans="1:7">
-      <c r="A41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="42" s="4" spans="1:7">
-      <c r="A42" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="43" s="4" spans="1:7">
-      <c r="A43" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="44" s="4" spans="1:7">
-      <c r="A44" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="45" s="4" spans="1:7">
-      <c r="A45" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="46" s="4" spans="1:7">
-      <c r="A46" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D46" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="47" s="4" spans="1:7">
-      <c r="A47" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D47" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="48" s="4" spans="1:7">
-      <c r="A48" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D48" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="49" s="4" spans="1:7">
-      <c r="A49" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="50" s="4" spans="1:7">
-      <c r="A50" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="51" s="4" spans="1:7">
-      <c r="A51" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="52" s="4" spans="1:7">
-      <c r="A52" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D52" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="53" s="4" spans="1:7">
-      <c r="A53" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D53" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="54" s="4" spans="1:7">
-      <c r="A54" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="55" s="4" spans="1:7">
-      <c r="A55" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="56" s="4" spans="1:7">
-      <c r="A56" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="57" s="4" spans="1:7">
-      <c r="A57" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D57" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="58" s="4" spans="1:7">
-      <c r="A58" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="59" s="4" spans="1:7">
-      <c r="A59" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D59" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="60" s="4" spans="1:7">
-      <c r="A60" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D60" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="61" s="4" spans="1:7">
-      <c r="A61" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D61" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="62" s="4" spans="1:7">
-      <c r="A62" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D62" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="63" s="4" spans="1:7">
-      <c r="A63" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D63" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="64" s="4" spans="1:7">
-      <c r="A64" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D64" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="65" s="4" spans="1:7">
-      <c r="A65" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D65" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="66" s="4" spans="1:7">
-      <c r="A66" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D66" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" t="s">
-        <v>190</v>
-      </c>
-      <c r="B67" t="s">
-        <v>191</v>
-      </c>
-      <c r="C67" t="s">
-        <v>192</v>
-      </c>
-      <c r="D67" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" t="s">
-        <v>193</v>
-      </c>
-      <c r="B68" t="s">
-        <v>194</v>
-      </c>
-      <c r="C68" t="s">
-        <v>195</v>
-      </c>
-      <c r="D68" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" t="s">
-        <v>196</v>
-      </c>
-      <c r="B69" t="s">
-        <v>197</v>
-      </c>
-      <c r="C69" t="s">
-        <v>198</v>
-      </c>
-      <c r="D69" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" t="s">
-        <v>199</v>
-      </c>
-      <c r="B70" t="s">
-        <v>200</v>
-      </c>
-      <c r="C70" t="s">
-        <v>201</v>
-      </c>
-      <c r="D70" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>202</v>
-      </c>
-      <c r="B71" t="s">
-        <v>203</v>
-      </c>
-      <c r="C71" t="s">
-        <v>204</v>
-      </c>
-      <c r="D71" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" t="s">
-        <v>205</v>
-      </c>
-      <c r="B72" t="s">
-        <v>206</v>
-      </c>
-      <c r="C72" t="s">
-        <v>207</v>
-      </c>
-      <c r="D72" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
-        <v>208</v>
-      </c>
-      <c r="B73" t="s">
-        <v>209</v>
-      </c>
-      <c r="C73" t="s">
-        <v>210</v>
-      </c>
-      <c r="D73" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" t="s">
-        <v>211</v>
-      </c>
-      <c r="B74" t="s">
-        <v>212</v>
-      </c>
-      <c r="C74" t="s">
-        <v>213</v>
-      </c>
-      <c r="D74" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" t="s">
-        <v>214</v>
-      </c>
-      <c r="B75" t="s">
-        <v>215</v>
-      </c>
-      <c r="C75" t="s">
-        <v>216</v>
-      </c>
-      <c r="D75" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>217</v>
-      </c>
-      <c r="B76" t="s">
-        <v>218</v>
-      </c>
-      <c r="C76" t="s">
-        <v>219</v>
-      </c>
-      <c r="D76" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>220</v>
-      </c>
-      <c r="B77" t="s">
-        <v>221</v>
-      </c>
-      <c r="C77" t="s">
-        <v>222</v>
-      </c>
-      <c r="D77" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" t="s">
-        <v>223</v>
-      </c>
-      <c r="B78" t="s">
-        <v>224</v>
-      </c>
-      <c r="C78" t="s">
-        <v>225</v>
-      </c>
-      <c r="D78" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" t="s">
-        <v>226</v>
-      </c>
-      <c r="B79" t="s">
-        <v>227</v>
-      </c>
-      <c r="C79" t="s">
-        <v>228</v>
-      </c>
-      <c r="D79" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
-        <v>229</v>
-      </c>
-      <c r="B80" t="s">
-        <v>230</v>
-      </c>
-      <c r="C80" t="s">
-        <v>231</v>
-      </c>
-      <c r="D80" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" t="s">
-        <v>232</v>
-      </c>
-      <c r="B81" t="s">
-        <v>233</v>
-      </c>
-      <c r="C81" t="s">
-        <v>234</v>
-      </c>
-      <c r="D81" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82" t="s">
-        <v>235</v>
-      </c>
-      <c r="B82" t="s">
-        <v>236</v>
-      </c>
-      <c r="C82" t="s">
-        <v>237</v>
-      </c>
-      <c r="D82" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83" t="s">
-        <v>238</v>
-      </c>
-      <c r="B83" t="s">
-        <v>239</v>
-      </c>
-      <c r="C83" t="s">
-        <v>240</v>
-      </c>
-      <c r="D83" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" t="s">
-        <v>241</v>
-      </c>
-      <c r="B84" t="s">
-        <v>242</v>
-      </c>
-      <c r="C84" t="s">
-        <v>243</v>
-      </c>
-      <c r="D84" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" t="s">
-        <v>244</v>
-      </c>
-      <c r="B85" t="s">
-        <v>245</v>
-      </c>
-      <c r="C85" t="s">
-        <v>246</v>
-      </c>
-      <c r="D85" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" t="s">
-        <v>247</v>
-      </c>
-      <c r="B86" t="s">
-        <v>248</v>
-      </c>
-      <c r="C86" t="s">
-        <v>249</v>
-      </c>
-      <c r="D86" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" t="s">
-        <v>250</v>
-      </c>
-      <c r="B87" t="s">
-        <v>251</v>
-      </c>
-      <c r="C87" t="s">
-        <v>252</v>
-      </c>
-      <c r="D87" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" t="s">
-        <v>253</v>
-      </c>
-      <c r="B88" t="s">
-        <v>254</v>
-      </c>
-      <c r="C88" t="s">
-        <v>255</v>
-      </c>
-      <c r="D88" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="A89" t="s">
-        <v>256</v>
-      </c>
-      <c r="B89" t="s">
-        <v>257</v>
-      </c>
-      <c r="C89" t="s">
-        <v>258</v>
-      </c>
-      <c r="D89" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" t="s">
-        <v>259</v>
-      </c>
-      <c r="B90" t="s">
-        <v>260</v>
-      </c>
-      <c r="C90" t="s">
-        <v>261</v>
-      </c>
-      <c r="D90" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="A91" t="s">
-        <v>262</v>
-      </c>
-      <c r="B91" t="s">
-        <v>263</v>
-      </c>
-      <c r="C91" t="s">
-        <v>264</v>
-      </c>
-      <c r="D91" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7">
-      <c r="A92" t="s">
-        <v>265</v>
-      </c>
-      <c r="D92" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
-      <c r="A93" t="s">
-        <v>266</v>
-      </c>
-      <c r="D93" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" t="s">
-        <v>267</v>
-      </c>
-      <c r="D94" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95" t="s">
-        <v>268</v>
-      </c>
-      <c r="B95" t="s">
-        <v>269</v>
-      </c>
-      <c r="C95" t="s">
-        <v>270</v>
-      </c>
-      <c r="D95" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96" t="s">
-        <v>271</v>
-      </c>
-      <c r="B96" t="s">
-        <v>272</v>
-      </c>
-      <c r="C96" t="s">
-        <v>273</v>
-      </c>
-      <c r="D96" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
-        <v>274</v>
-      </c>
-      <c r="B97" t="s">
-        <v>275</v>
-      </c>
-      <c r="C97" t="s">
-        <v>276</v>
-      </c>
-      <c r="D97" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
-        <v>277</v>
-      </c>
-      <c r="B98" t="s">
-        <v>278</v>
-      </c>
-      <c r="C98" t="s">
-        <v>279</v>
-      </c>
-      <c r="D98" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
-        <v>280</v>
-      </c>
-      <c r="B99" t="s">
-        <v>281</v>
-      </c>
-      <c r="C99" t="s">
-        <v>282</v>
-      </c>
-      <c r="D99" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" t="s">
-        <v>283</v>
-      </c>
-      <c r="B100" t="s">
-        <v>284</v>
-      </c>
-      <c r="C100" t="s">
-        <v>285</v>
-      </c>
-      <c r="D100" t="n">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="25"/>
+    <col min="1" max="1" width="25" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="19" r="1" s="4" spans="1:2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:2" ht="19" customHeight="1">
+      <c r="A1" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>286</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="5" t="n">
-        <v>42583</v>
-      </c>
-      <c r="B2" t="n">
-        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3588,11 +3839,16 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <f>SUM(Sheet!G2:G100)</f>
-        <v/>
+        <f>SUM(Sheet!E2:E113)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created auto email timer and improved performance
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="1"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Monthly_STAT" sheetId="2" r:id="rId2"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" activeTab="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthly_STAT" sheetId="2" r:id="rId2"/>
+  </sheets>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="370">
   <si>
     <t>UID</t>
   </si>
@@ -30,6 +35,9 @@
   </si>
   <si>
     <t>September 2016</t>
+  </si>
+  <si>
+    <t>October 2016</t>
   </si>
   <si>
     <t>8FD8AAE4A0</t>
@@ -1127,45 +1135,31 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color indexed="8"/>
-      <sz val="12"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="18"/>
     </font>
     <font>
+      <i/>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <i val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="15"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="18"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <i val="1"/>
-      <color rgb="00000000"/>
-      <sz val="15"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -1202,24 +1196,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="49" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="49" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -2395,35 +2389,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E131"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IE131"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="20"/>
-    <col customWidth="1" max="3" min="2" style="4" width="30"/>
-    <col customWidth="1" max="3" min="3" style="4" width="30"/>
-    <col customWidth="1" max="246" min="4" style="4" width="20"/>
-    <col customWidth="1" max="5" min="5" style="4" width="20"/>
-    <col customWidth="1" max="6" min="6" style="4" width="20"/>
+    <col min="1" max="1" width="20" style="4" customWidth="1"/>
+    <col min="2" max="3" width="30" style="4" customWidth="1"/>
+    <col min="4" max="239" width="20" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="23" r="1" s="4" spans="1:5">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" ht="23" customHeight="1">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -2432,2011 +2419,2015 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row customHeight="1" ht="17" r="2" s="4" spans="1:5">
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="F2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>6</v>
+      </c>
+      <c r="E3">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="17" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2">
+        <v>13</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" customHeight="1">
+      <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2">
+        <v>43</v>
+      </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" customHeight="1">
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5</v>
+      </c>
+      <c r="E21">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="n"/>
-      <c r="D2" s="3" t="n"/>
-    </row>
-    <row customHeight="1" ht="17" r="3" s="4" spans="1:5">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="22" spans="1:5" ht="17" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="2">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" s="2">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="n">
+    </row>
+    <row r="28" spans="1:5" ht="17" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="17" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="2">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="17" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="17" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="2">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="17" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="17" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17" customHeight="1">
+      <c r="A37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+      <c r="E37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="17" customHeight="1">
+      <c r="A38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="2">
         <v>6</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="17" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="2">
+        <v>7</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="17" customHeight="1">
+      <c r="A40" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="2">
+        <v>4</v>
+      </c>
+      <c r="E40">
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="4" s="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="5" s="4" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="n">
+    <row r="41" spans="1:5" ht="17" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="17" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="17" customHeight="1">
+      <c r="A43" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17" customHeight="1">
+      <c r="A44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="17" customHeight="1">
+      <c r="A45" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="2">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E45">
         <v>5</v>
       </c>
     </row>
-    <row customHeight="1" ht="17" r="6" s="4" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" t="n">
+    <row r="46" spans="1:5" ht="17" customHeight="1">
+      <c r="A46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17" customHeight="1">
+      <c r="A47" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="2">
+        <v>3</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="17" customHeight="1">
+      <c r="A48" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="2">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row customHeight="1" ht="17" r="7" s="4" spans="1:5">
-      <c r="A7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="n"/>
-      <c r="D7" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="8" s="4" spans="1:5">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="3" t="n"/>
-      <c r="E8" t="n">
+      <c r="E49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="17" customHeight="1">
+      <c r="A50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="2">
+        <v>4</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" customHeight="1">
+      <c r="A51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row customHeight="1" ht="17" r="9" s="4" spans="1:5">
-      <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2" t="n">
+      <c r="E51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="17" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row customHeight="1" ht="17" r="10" s="4" spans="1:5">
-      <c r="A10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E10" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="11" s="4" spans="1:5">
-      <c r="A11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="E11" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="12" s="4" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" t="n">
+      <c r="E52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="17" customHeight="1">
+      <c r="A53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="17" customHeight="1">
+      <c r="A54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="2">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="17" customHeight="1">
+      <c r="A55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row customHeight="1" ht="17" r="13" s="4" spans="1:5">
-      <c r="A13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3" t="n">
+      <c r="E55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" customHeight="1">
+      <c r="A56" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="2">
         <v>3</v>
       </c>
-      <c r="E13" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="14" s="4" spans="1:5">
-      <c r="A14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>43</v>
-      </c>
-      <c r="E14" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="15" s="4" spans="1:5">
-      <c r="A15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="E15" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="16" s="4" spans="1:5">
-      <c r="A16" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E16" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="17" s="4" spans="1:5">
-      <c r="A17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E17" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="18" s="4" spans="1:5">
-      <c r="A18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E18" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="19" s="4" spans="1:5">
-      <c r="A19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="20" s="4" spans="1:5">
-      <c r="A20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="3" t="n"/>
-      <c r="D20" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="21" s="4" spans="1:5">
-      <c r="A21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E21" t="n">
+    </row>
+    <row r="57" spans="1:5" ht="17" customHeight="1">
+      <c r="A57" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D57" s="2">
+        <v>2</v>
+      </c>
+      <c r="E57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" customHeight="1">
+      <c r="A58" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" customHeight="1">
+      <c r="A59" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row customHeight="1" ht="17" r="22" s="4" spans="1:5">
-      <c r="A22" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E22" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="23" s="4" spans="1:5">
-      <c r="A23" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" s="2" t="n">
+      <c r="E59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17" customHeight="1">
+      <c r="A60" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" customHeight="1">
+      <c r="A61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" s="2">
         <v>3</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" customHeight="1">
+      <c r="A62" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D62" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" customHeight="1">
+      <c r="A63" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D63" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" customHeight="1">
+      <c r="A64" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" s="2">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" customHeight="1">
+      <c r="A65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D65" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" customHeight="1">
+      <c r="A66" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D66" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row customHeight="1" ht="17" r="24" s="4" spans="1:5">
-      <c r="A24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="25" s="4" spans="1:5">
-      <c r="A25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="26" s="4" spans="1:5">
-      <c r="A26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="27" s="4" spans="1:5">
-      <c r="A27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="28" s="4" spans="1:5">
-      <c r="A28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E28" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="29" s="4" spans="1:5">
-      <c r="A29" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E29" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="30" s="4" spans="1:5">
-      <c r="A30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="31" s="4" spans="1:5">
-      <c r="A31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E31" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="32" s="4" spans="1:5">
-      <c r="A32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E32" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="33" s="4" spans="1:5">
-      <c r="A33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="34" s="4" spans="1:5">
-      <c r="A34" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="E34" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="35" s="4" spans="1:5">
-      <c r="A35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E35" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="36" s="4" spans="1:5">
-      <c r="A36" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D36" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E36" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="37" s="4" spans="1:5">
-      <c r="A37" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D37" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E37" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="38" s="4" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D38" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E38" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="39" s="4" spans="1:5">
-      <c r="A39" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E39" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="40" s="4" spans="1:5">
-      <c r="A40" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D40" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E40" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="41" s="4" spans="1:5">
-      <c r="A41" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E41" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="42" s="4" spans="1:5">
-      <c r="A42" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D42" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="43" s="4" spans="1:5">
-      <c r="A43" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="44" s="4" spans="1:5">
-      <c r="A44" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D44" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="45" s="4" spans="1:5">
-      <c r="A45" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D45" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E45" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="46" s="4" spans="1:5">
-      <c r="A46" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D46" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="47" s="4" spans="1:5">
-      <c r="A47" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="48" s="4" spans="1:5">
-      <c r="A48" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D48" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E48" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="49" s="4" spans="1:5">
-      <c r="A49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D49" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E49" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="50" s="4" spans="1:5">
-      <c r="A50" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D50" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E50" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="51" s="4" spans="1:5">
-      <c r="A51" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D51" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E51" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="52" s="4" spans="1:5">
-      <c r="A52" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D52" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E52" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="53" s="4" spans="1:5">
-      <c r="A53" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D53" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="54" s="4" spans="1:5">
-      <c r="A54" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D54" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E54" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="55" s="4" spans="1:5">
-      <c r="A55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D55" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="E55" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="56" s="4" spans="1:5">
-      <c r="A56" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D56" s="2" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="57" s="4" spans="1:5">
-      <c r="A57" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D57" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="E57" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="58" s="4" spans="1:5">
-      <c r="A58" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D58" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="59" s="4" spans="1:5">
-      <c r="A59" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E59" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="60" s="4" spans="1:5">
-      <c r="A60" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D60" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="61" s="4" spans="1:5">
-      <c r="A61" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D61" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E61" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="62" s="4" spans="1:5">
-      <c r="A62" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D62" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="63" s="4" spans="1:5">
-      <c r="A63" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D63" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="64" s="4" spans="1:5">
-      <c r="A64" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D64" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E64" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="65" s="4" spans="1:5">
-      <c r="A65" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D65" s="2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="17" r="66" s="4" spans="1:5">
-      <c r="A66" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D66" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E66" t="n">
+      <c r="E66">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B67" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C67" t="s">
-        <v>197</v>
-      </c>
-      <c r="D67" t="n">
+        <v>198</v>
+      </c>
+      <c r="D67">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C68" t="s">
-        <v>200</v>
-      </c>
-      <c r="D68" t="n">
+        <v>201</v>
+      </c>
+      <c r="D68">
         <v>4</v>
       </c>
-      <c r="E68" t="n">
+      <c r="E68">
         <v>4</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B69" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C69" t="s">
-        <v>203</v>
-      </c>
-      <c r="D69" t="n">
+        <v>204</v>
+      </c>
+      <c r="D69">
         <v>8</v>
       </c>
-      <c r="E69" t="n">
+      <c r="E69">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B70" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C70" t="s">
-        <v>206</v>
-      </c>
-      <c r="D70" t="n">
+        <v>207</v>
+      </c>
+      <c r="D70">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B71" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C71" t="s">
-        <v>209</v>
-      </c>
-      <c r="D71" t="n">
+        <v>210</v>
+      </c>
+      <c r="D71">
         <v>3</v>
       </c>
-      <c r="E71" t="n">
+      <c r="E71">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B72" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C72" t="s">
-        <v>212</v>
-      </c>
-      <c r="D72" t="n">
+        <v>213</v>
+      </c>
+      <c r="D72">
         <v>3</v>
       </c>
-      <c r="E72" t="n">
+      <c r="E72">
         <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B73" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C73" t="s">
-        <v>215</v>
-      </c>
-      <c r="D73" t="n">
+        <v>216</v>
+      </c>
+      <c r="D73">
         <v>3</v>
       </c>
-      <c r="E73" t="n">
+      <c r="E73">
         <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C74" t="s">
-        <v>218</v>
-      </c>
-      <c r="D74" t="n">
+        <v>219</v>
+      </c>
+      <c r="D74">
         <v>8</v>
       </c>
-      <c r="E74" t="n">
+      <c r="E74">
         <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B75" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C75" t="s">
-        <v>221</v>
-      </c>
-      <c r="D75" t="n">
+        <v>222</v>
+      </c>
+      <c r="D75">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B76" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C76" t="s">
-        <v>224</v>
-      </c>
-      <c r="D76" t="n">
+        <v>225</v>
+      </c>
+      <c r="D76">
         <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B77" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C77" t="s">
-        <v>227</v>
-      </c>
-      <c r="D77" t="n">
+        <v>228</v>
+      </c>
+      <c r="D77">
         <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B78" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C78" t="s">
-        <v>230</v>
-      </c>
-      <c r="D78" t="n">
+        <v>231</v>
+      </c>
+      <c r="D78">
         <v>3</v>
       </c>
-      <c r="E78" t="n">
+      <c r="E78">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B79" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C79" t="s">
-        <v>233</v>
-      </c>
-      <c r="D79" t="n">
+        <v>234</v>
+      </c>
+      <c r="D79">
         <v>3</v>
       </c>
-      <c r="E79" t="n">
+      <c r="E79">
         <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B80" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C80" t="s">
-        <v>236</v>
-      </c>
-      <c r="D80" t="n">
+        <v>237</v>
+      </c>
+      <c r="D80">
         <v>3</v>
       </c>
-      <c r="E80" t="n">
+      <c r="E80">
         <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B81" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C81" t="s">
-        <v>239</v>
-      </c>
-      <c r="D81" t="n">
+        <v>240</v>
+      </c>
+      <c r="D81">
         <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B82" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C82" t="s">
-        <v>242</v>
-      </c>
-      <c r="D82" t="n">
-        <v>1</v>
-      </c>
-      <c r="E82" t="n">
+        <v>243</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+      <c r="E82">
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B83" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C83" t="s">
-        <v>245</v>
-      </c>
-      <c r="D83" t="n">
-        <v>1</v>
-      </c>
-      <c r="E83" t="n">
+        <v>246</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83">
         <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B84" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C84" t="s">
-        <v>248</v>
-      </c>
-      <c r="D84" t="n">
-        <v>1</v>
-      </c>
-      <c r="E84" t="n">
+        <v>249</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B85" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C85" t="s">
-        <v>251</v>
-      </c>
-      <c r="D85" t="n">
+        <v>252</v>
+      </c>
+      <c r="D85">
         <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B86" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C86" t="s">
-        <v>254</v>
-      </c>
-      <c r="D86" t="n">
+        <v>255</v>
+      </c>
+      <c r="D86">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B87" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C87" t="s">
-        <v>257</v>
-      </c>
-      <c r="D87" t="n">
-        <v>2</v>
-      </c>
-      <c r="E87" t="n">
+        <v>258</v>
+      </c>
+      <c r="D87">
+        <v>2</v>
+      </c>
+      <c r="E87">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B88" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C88" t="s">
-        <v>260</v>
-      </c>
-      <c r="D88" t="n">
-        <v>1</v>
-      </c>
-      <c r="E88" t="n">
+        <v>261</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+      <c r="E88">
         <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B89" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C89" t="s">
-        <v>263</v>
-      </c>
-      <c r="D89" t="n">
+        <v>264</v>
+      </c>
+      <c r="D89">
         <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B90" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C90" t="s">
-        <v>266</v>
-      </c>
-      <c r="D90" t="n">
+        <v>267</v>
+      </c>
+      <c r="D90">
         <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B91" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C91" t="s">
-        <v>269</v>
-      </c>
-      <c r="D91" t="n">
+        <v>270</v>
+      </c>
+      <c r="D91">
         <v>4</v>
       </c>
-      <c r="E91" t="n">
+      <c r="E91">
         <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>270</v>
-      </c>
-      <c r="D92" t="n">
+        <v>271</v>
+      </c>
+      <c r="D92">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>271</v>
-      </c>
-      <c r="D93" t="n">
-        <v>1</v>
-      </c>
-      <c r="E93" t="n">
+        <v>272</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>272</v>
-      </c>
-      <c r="D94" t="n">
+        <v>273</v>
+      </c>
+      <c r="D94">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B95" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C95" t="s">
-        <v>275</v>
-      </c>
-      <c r="D95" t="n">
+        <v>276</v>
+      </c>
+      <c r="D95">
         <v>3</v>
       </c>
-      <c r="E95" t="n">
+      <c r="E95">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B96" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C96" t="s">
-        <v>278</v>
-      </c>
-      <c r="D96" t="n">
-        <v>2</v>
-      </c>
-      <c r="E96" t="n">
+        <v>279</v>
+      </c>
+      <c r="D96">
+        <v>2</v>
+      </c>
+      <c r="E96">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B97" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C97" t="s">
-        <v>281</v>
-      </c>
-      <c r="D97" t="n">
-        <v>1</v>
-      </c>
-      <c r="E97" t="n">
+        <v>282</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+      <c r="E97">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B98" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C98" t="s">
-        <v>284</v>
-      </c>
-      <c r="D98" t="n">
+        <v>285</v>
+      </c>
+      <c r="D98">
         <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B99" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C99" t="s">
-        <v>287</v>
-      </c>
-      <c r="D99" t="n">
+        <v>288</v>
+      </c>
+      <c r="D99">
         <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B100" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C100" t="s">
-        <v>290</v>
-      </c>
-      <c r="D100" t="n">
+        <v>291</v>
+      </c>
+      <c r="D100">
         <v>3</v>
       </c>
-      <c r="E100" t="n">
+      <c r="E100">
         <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B101" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C101" t="s">
-        <v>293</v>
-      </c>
-      <c r="D101" t="n">
-        <v>1</v>
-      </c>
-      <c r="E101" t="n">
+        <v>294</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101">
         <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>294</v>
-      </c>
-      <c r="D102" t="n">
+        <v>295</v>
+      </c>
+      <c r="D102">
         <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B103" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C103" t="s">
-        <v>297</v>
-      </c>
-      <c r="D103" t="n">
+        <v>298</v>
+      </c>
+      <c r="D103">
         <v>4</v>
       </c>
-      <c r="E103" t="n">
+      <c r="E103">
         <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B104" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C104" t="s">
-        <v>300</v>
-      </c>
-      <c r="D104" t="n">
-        <v>2</v>
-      </c>
-      <c r="E104" t="n">
+        <v>301</v>
+      </c>
+      <c r="D104">
+        <v>2</v>
+      </c>
+      <c r="E104">
         <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B105" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C105" t="s">
-        <v>303</v>
-      </c>
-      <c r="D105" t="n">
+        <v>304</v>
+      </c>
+      <c r="D105">
         <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B106" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C106" t="s">
-        <v>306</v>
-      </c>
-      <c r="D106" t="n">
-        <v>2</v>
-      </c>
-      <c r="E106" t="n">
+        <v>307</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B107" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C107" t="s">
-        <v>309</v>
-      </c>
-      <c r="D107" t="n">
-        <v>2</v>
-      </c>
-      <c r="E107" t="n">
+        <v>310</v>
+      </c>
+      <c r="D107">
+        <v>2</v>
+      </c>
+      <c r="E107">
         <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B108" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C108" t="s">
-        <v>312</v>
-      </c>
-      <c r="D108" t="n">
+        <v>313</v>
+      </c>
+      <c r="D108">
         <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B109" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C109" t="s">
-        <v>315</v>
-      </c>
-      <c r="D109" t="n">
+        <v>316</v>
+      </c>
+      <c r="D109">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B110" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C110" t="s">
-        <v>318</v>
-      </c>
-      <c r="D110" t="n">
-        <v>2</v>
-      </c>
-      <c r="E110" t="n">
+        <v>319</v>
+      </c>
+      <c r="D110">
+        <v>2</v>
+      </c>
+      <c r="E110">
         <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B111" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C111" t="s">
-        <v>321</v>
-      </c>
-      <c r="D111" t="n">
-        <v>2</v>
-      </c>
-      <c r="E111" t="n">
+        <v>322</v>
+      </c>
+      <c r="D111">
+        <v>2</v>
+      </c>
+      <c r="E111">
         <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B112" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C112" t="s">
-        <v>324</v>
-      </c>
-      <c r="D112" t="n">
-        <v>2</v>
-      </c>
-      <c r="E112" t="n">
+        <v>325</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="E112">
         <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B113" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C113" t="s">
-        <v>327</v>
-      </c>
-      <c r="D113" t="n">
-        <v>1</v>
-      </c>
-      <c r="E113" t="n">
+        <v>328</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113">
         <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B114" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C114" t="s">
-        <v>330</v>
-      </c>
-      <c r="E114" t="n">
+        <v>331</v>
+      </c>
+      <c r="E114">
         <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>331</v>
-      </c>
-      <c r="E115" t="n">
+        <v>332</v>
+      </c>
+      <c r="E115">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>332</v>
-      </c>
-      <c r="E116" t="n">
+        <v>333</v>
+      </c>
+      <c r="E116">
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>333</v>
-      </c>
-      <c r="E117" t="n">
+        <v>334</v>
+      </c>
+      <c r="E117">
         <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B118" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C118" t="s">
-        <v>336</v>
-      </c>
-      <c r="E118" t="n">
+        <v>337</v>
+      </c>
+      <c r="E118">
         <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>337</v>
-      </c>
-      <c r="E119" t="n">
+        <v>338</v>
+      </c>
+      <c r="E119">
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>338</v>
-      </c>
-      <c r="E120" t="n">
+        <v>339</v>
+      </c>
+      <c r="E120">
         <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
-        <v>339</v>
-      </c>
-      <c r="E121" t="n">
+        <v>340</v>
+      </c>
+      <c r="E121">
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B122" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C122" t="s">
-        <v>342</v>
-      </c>
-      <c r="E122" t="n">
+        <v>343</v>
+      </c>
+      <c r="E122">
         <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
-        <v>343</v>
-      </c>
-      <c r="E123" t="n">
+        <v>344</v>
+      </c>
+      <c r="E123">
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B124" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C124" t="s">
-        <v>346</v>
-      </c>
-      <c r="E124" t="n">
+        <v>347</v>
+      </c>
+      <c r="E124">
         <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B125" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C125" t="s">
-        <v>349</v>
-      </c>
-      <c r="E125" t="n">
+        <v>350</v>
+      </c>
+      <c r="E125">
         <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B126" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C126" t="s">
-        <v>352</v>
-      </c>
-      <c r="E126" t="n">
+        <v>353</v>
+      </c>
+      <c r="E126">
         <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B127" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C127" t="s">
-        <v>355</v>
-      </c>
-      <c r="E127" t="n">
+        <v>356</v>
+      </c>
+      <c r="E127">
         <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B128" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C128" t="s">
-        <v>358</v>
-      </c>
-      <c r="E128" t="n">
+        <v>359</v>
+      </c>
+      <c r="E128">
         <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:5">
       <c r="A129" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B129" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C129" t="s">
-        <v>361</v>
-      </c>
-      <c r="E129" t="n">
+        <v>362</v>
+      </c>
+      <c r="E129">
         <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:5">
       <c r="A130" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B130" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C130" t="s">
-        <v>364</v>
-      </c>
-      <c r="E130" t="n">
+        <v>365</v>
+      </c>
+      <c r="E130">
         <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:5">
       <c r="A131" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="B131" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C131" t="s">
-        <v>367</v>
-      </c>
-      <c r="E131" t="n">
+        <v>368</v>
+      </c>
+      <c r="E131">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="4" width="25"/>
+    <col min="1" max="1" width="25" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="19" r="1" s="4" spans="1:2">
+    <row r="1" spans="1:2" ht="19" customHeight="1">
       <c r="A1" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="n">
-        <v>286</v>
+      <c r="A2" s="6">
+        <v>42583</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4444,11 +4435,15 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <f>SUM(Sheet!E2:E131)</f>
-        <v/>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ready for full program testing
</commit_message>
<xml_diff>
--- a/testing.xlsx
+++ b/testing.xlsx
@@ -3381,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row customHeight="1" ht="17" r="15" s="4" spans="1:9">
@@ -7128,23 +7128,36 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="n">
-        <v>286</v>
+      <c r="B2">
+        <f>SUM(Sheet!D2:D222)</f>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <f>SUM(Sheet!E2:E222)</f>
+        <v/>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4">
+        <f>SUM(Sheet!F2:F222)</f>
+        <v/>
+      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
+      </c>
+      <c r="B5">
+        <f>SUM(Sheet!G2:G222)</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:2">

</xml_diff>